<commit_message>
Definindo tipos e validação de dados das colunas
</commit_message>
<xml_diff>
--- a/bases/base de estoque.xlsx
+++ b/bases/base de estoque.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leo\Desktop\controleEstoque\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE43634-0986-4041-99B5-C8215C08E2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68E7409-EE31-4A60-BFF3-5F912880B479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,15 +71,9 @@
     <t>Data</t>
   </si>
   <si>
-    <t>Tipo de Movimentação(Entrada/Saída/Ajuste)</t>
-  </si>
-  <si>
     <t>Quantidade</t>
   </si>
   <si>
-    <t>Motivo(venda/devolução/perda/reposição/etc</t>
-  </si>
-  <si>
     <t>Observações</t>
   </si>
   <si>
@@ -92,9 +86,6 @@
     <t>Quantidade atual</t>
   </si>
   <si>
-    <t>Status (OK/Atenção/Criticidade)</t>
-  </si>
-  <si>
     <t>Valor total em estoque</t>
   </si>
   <si>
@@ -108,13 +99,25 @@
   </si>
   <si>
     <t>Custo estimado de compra</t>
+  </si>
+  <si>
+    <t>Tipo de Movimentação</t>
+  </si>
+  <si>
+    <t>Motivo</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,6 +127,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -146,16 +156,89 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="22">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -172,30 +255,30 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E0BFA38-6908-4083-9EDE-210C6043F638}" name="Tabela1" displayName="Tabela1" ref="D3:K14">
   <autoFilter ref="D3:K14" xr:uid="{2E0BFA38-6908-4083-9EDE-210C6043F638}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{E8D6F2E1-8A24-43F9-99A0-29DA8BE6B489}" name="Código do Produto" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{5A178A17-5607-486B-9A86-2749B65D3235}" name="Nome"/>
-    <tableColumn id="3" xr3:uid="{830840EC-1BFC-450C-A210-9D4BC7F3B359}" name="Categoria"/>
-    <tableColumn id="4" xr3:uid="{51DEA236-4788-4C97-B298-70CA221638B3}" name="Unidade de medida"/>
-    <tableColumn id="5" xr3:uid="{43D7FCB4-0C38-4BD5-B01F-E5AAAB08DB90}" name="Fornecedor"/>
-    <tableColumn id="6" xr3:uid="{CC9B98B4-BFAD-4372-9C2F-7913D52ED9DC}" name="Preço de custo"/>
-    <tableColumn id="7" xr3:uid="{12E1A6A2-CECB-4190-965D-99C38CE8672F}" name="Estoque mínimo"/>
-    <tableColumn id="8" xr3:uid="{EDC57470-16BA-42D3-BDF0-B2168563FDB4}" name="Estoque máximo" totalsRowFunction="count"/>
+    <tableColumn id="1" xr3:uid="{E8D6F2E1-8A24-43F9-99A0-29DA8BE6B489}" name="Código do Produto" totalsRowLabel="Total" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{5A178A17-5607-486B-9A86-2749B65D3235}" name="Nome" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{830840EC-1BFC-450C-A210-9D4BC7F3B359}" name="Categoria" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{51DEA236-4788-4C97-B298-70CA221638B3}" name="Unidade de medida" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{43D7FCB4-0C38-4BD5-B01F-E5AAAB08DB90}" name="Fornecedor" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{CC9B98B4-BFAD-4372-9C2F-7913D52ED9DC}" name="Preço de custo" dataCellStyle="Moeda"/>
+    <tableColumn id="7" xr3:uid="{12E1A6A2-CECB-4190-965D-99C38CE8672F}" name="Estoque mínimo" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{EDC57470-16BA-42D3-BDF0-B2168563FDB4}" name="Estoque máximo" totalsRowFunction="count" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{ED9732E9-C816-4C9A-B4F0-EB0D9BDE2EE7}" name="Tabela2" displayName="Tabela2" ref="C3:I15" totalsRowShown="0">
-  <autoFilter ref="C3:I15" xr:uid="{ED9732E9-C816-4C9A-B4F0-EB0D9BDE2EE7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{ED9732E9-C816-4C9A-B4F0-EB0D9BDE2EE7}" name="Tabela2" displayName="Tabela2" ref="D3:J15" totalsRowShown="0">
+  <autoFilter ref="D3:J15" xr:uid="{ED9732E9-C816-4C9A-B4F0-EB0D9BDE2EE7}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{5EB596D3-13E5-41DA-B68D-330423824A6E}" name="Data"/>
-    <tableColumn id="2" xr3:uid="{D03F4BD6-5A38-46FF-A002-2C7AE24A1554}" name="Tipo de Movimentação(Entrada/Saída/Ajuste)"/>
-    <tableColumn id="3" xr3:uid="{7F37AC3D-3B5E-49EE-B9C8-D9AFFAA48E5F}" name="Código do Produto"/>
-    <tableColumn id="4" xr3:uid="{FC5DF69A-2251-49E2-802C-C0E01E71C254}" name="Quantidade"/>
-    <tableColumn id="5" xr3:uid="{9C283E40-D88C-48C9-B447-391D9424BE74}" name="Motivo(venda/devolução/perda/reposição/etc"/>
-    <tableColumn id="6" xr3:uid="{A72EC6A0-3612-4E93-803B-D3A43885D305}" name="Responsáveis"/>
-    <tableColumn id="7" xr3:uid="{DD2075B4-09AE-4DFA-83E3-E8DF20084BD7}" name="Observações"/>
+    <tableColumn id="1" xr3:uid="{5EB596D3-13E5-41DA-B68D-330423824A6E}" name="Data" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{D03F4BD6-5A38-46FF-A002-2C7AE24A1554}" name="Tipo de Movimentação" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{7F37AC3D-3B5E-49EE-B9C8-D9AFFAA48E5F}" name="Código do Produto" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{FC5DF69A-2251-49E2-802C-C0E01E71C254}" name="Quantidade" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{9C283E40-D88C-48C9-B447-391D9424BE74}" name="Motivo" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{A72EC6A0-3612-4E93-803B-D3A43885D305}" name="Responsáveis" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{DD2075B4-09AE-4DFA-83E3-E8DF20084BD7}" name="Observações" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -205,11 +288,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5DB4A4AD-109D-4C62-B581-EC74E8DF7B36}" name="Tabela4" displayName="Tabela4" ref="D3:H15" totalsRowShown="0">
   <autoFilter ref="D3:H15" xr:uid="{5DB4A4AD-109D-4C62-B581-EC74E8DF7B36}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{296C906F-86E1-4C3F-87AC-3BB0690DFCB5}" name="Lista de itens abaixo do estoque mínimo"/>
-    <tableColumn id="2" xr3:uid="{49797186-5174-4105-9BDC-28152E70824C}" name="Quantidade sugerida para compra"/>
-    <tableColumn id="3" xr3:uid="{06C6B836-5CE8-4814-83AA-437570C11F20}" name="Fornecedor"/>
+    <tableColumn id="1" xr3:uid="{296C906F-86E1-4C3F-87AC-3BB0690DFCB5}" name="Lista de itens abaixo do estoque mínimo" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{49797186-5174-4105-9BDC-28152E70824C}" name="Quantidade sugerida para compra" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{06C6B836-5CE8-4814-83AA-437570C11F20}" name="Fornecedor" dataDxfId="5"/>
     <tableColumn id="4" xr3:uid="{AFF0190F-635E-452E-8997-7BB69297B3D2}" name="Lead time"/>
-    <tableColumn id="5" xr3:uid="{8FA2F226-83F8-431D-B33F-23C6772A656C}" name="Custo estimado de compra"/>
+    <tableColumn id="5" xr3:uid="{8FA2F226-83F8-431D-B33F-23C6772A656C}" name="Custo estimado de compra" dataCellStyle="Moeda"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -219,12 +302,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2161A2C0-C6F9-4249-A25F-86E29D708A19}" name="Tabela3" displayName="Tabela3" ref="D3:I15" totalsRowShown="0">
   <autoFilter ref="D3:I15" xr:uid="{2161A2C0-C6F9-4249-A25F-86E29D708A19}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{B1F0DD55-3D0C-436D-BD4F-30A9F86588D8}" name="Código do Produto"/>
-    <tableColumn id="2" xr3:uid="{D60E5A99-FCE6-4BB6-B5C6-CF533E9E7674}" name="Nome do Produto"/>
-    <tableColumn id="3" xr3:uid="{EAF9CB50-13B7-40D1-A0D8-4519F7739BCF}" name="Quantidade atual"/>
-    <tableColumn id="4" xr3:uid="{4200BEDB-FC2D-4A30-8DBB-31920E9A30CB}" name="Estoque mínimo"/>
-    <tableColumn id="5" xr3:uid="{6484B93B-1AB3-42A1-9062-78CA337C1E56}" name="Status (OK/Atenção/Criticidade)"/>
-    <tableColumn id="6" xr3:uid="{28B842BE-778A-4EE6-8D3E-AA6F96CF9BD2}" name="Valor total em estoque"/>
+    <tableColumn id="1" xr3:uid="{B1F0DD55-3D0C-436D-BD4F-30A9F86588D8}" name="Código do Produto" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{D60E5A99-FCE6-4BB6-B5C6-CF533E9E7674}" name="Nome do Produto" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{EAF9CB50-13B7-40D1-A0D8-4519F7739BCF}" name="Quantidade atual" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{4200BEDB-FC2D-4A30-8DBB-31920E9A30CB}" name="Estoque mínimo" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{6484B93B-1AB3-42A1-9062-78CA337C1E56}" name="Status" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{28B842BE-778A-4EE6-8D3E-AA6F96CF9BD2}" name="Valor total em estoque" dataCellStyle="Moeda"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -493,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D3:K3"/>
+  <dimension ref="D3:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,6 +621,116 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -549,47 +742,164 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08727648-F844-49B9-80D8-34C885ED1FA4}">
-  <dimension ref="C3:I3"/>
+  <dimension ref="D3:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="7.140625" customWidth="1"/>
-    <col min="4" max="4" width="43.42578125" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" customWidth="1"/>
-    <col min="7" max="7" width="44.5703125" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+    <row r="3" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" t="s">
         <v>10</v>
       </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" t="s">
-        <v>12</v>
-      </c>
+    </row>
+    <row r="4" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D4" s="4"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D5" s="4"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D6" s="4"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D7" s="4"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D8" s="4"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D9" s="4"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D10" s="4"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D11" s="4"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D12" s="4"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D13" s="4"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D14" s="4"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D15" s="4"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E15" xr:uid="{703E9282-576D-4A9A-A218-19CF88794E67}">
+      <formula1>"Entrada,Saída,Ajuste"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H15" xr:uid="{CF5DC616-8130-4BB1-A2BE-78591D8EBC91}">
+      <formula1>"Venda,Devolução,Perda,Reposição"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -599,37 +909,110 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47C9561B-5C31-4F54-9526-8B42AEE30216}">
-  <dimension ref="D3:H3"/>
+  <dimension ref="D3:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="38.5703125" customWidth="1"/>
-    <col min="5" max="5" width="32.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1"/>
-    <col min="8" max="8" width="26.5703125" customWidth="1"/>
+    <col min="1" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
         <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
-      </c>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D4" s="1"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="1"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D5" s="1"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="1"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D6" s="1"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="1"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D7" s="1"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="1"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D8" s="1"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="1"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D9" s="1"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="1"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D10" s="1"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="1"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D11" s="1"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="1"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D12" s="1"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="1"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D13" s="1"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="1"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D14" s="1"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="1"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D15" s="1"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="1"/>
+      <c r="H15" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -641,20 +1024,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6F0B329-A77C-4A09-A2FE-86C78D1F79E7}">
-  <dimension ref="D3:I3"/>
+  <dimension ref="D3:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="1" max="3" width="6.7109375" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="31.5703125" customWidth="1"/>
-    <col min="8" max="8" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="4:9" x14ac:dyDescent="0.25">
@@ -662,22 +1046,123 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s">
         <v>6</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="I3" t="s">
-        <v>17</v>
-      </c>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="2"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H15" xr:uid="{2925EAA5-0E84-400E-8FE6-5764D6680FD2}">
+      <formula1>"OK,Atenção,Crítico"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Congelamento de painéis das abas
</commit_message>
<xml_diff>
--- a/bases/base de estoque.xlsx
+++ b/bases/base de estoque.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leo\Desktop\controleEstoque\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5856EA6B-8BE7-4C67-A76F-0AF0886A8DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE3A9772-F090-4DEB-A0FD-DA08533F7119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cadastro" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Código do Produto</t>
   </si>
@@ -98,28 +98,10 @@
     <t>Tipo de Movimentação</t>
   </si>
   <si>
-    <t>Entrada</t>
-  </si>
-  <si>
     <t>Motivo</t>
   </si>
   <si>
     <t>Status</t>
-  </si>
-  <si>
-    <t>OK</t>
-  </si>
-  <si>
-    <t>Atenção</t>
-  </si>
-  <si>
-    <t>Crítico</t>
-  </si>
-  <si>
-    <t>Saída</t>
-  </si>
-  <si>
-    <t>Ajuste</t>
   </si>
   <si>
     <t>Movimentações</t>
@@ -1658,7 +1640,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BB17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1734,7 +1719,7 @@
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="8" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -1994,7 +1979,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08727648-F844-49B9-80D8-34C885ED1FA4}">
   <dimension ref="A1:BB18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2069,7 +2057,7 @@
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="8" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -2193,7 +2181,7 @@
         <v>9</v>
       </c>
       <c r="I6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J6" t="s">
         <v>11</v>
@@ -2204,9 +2192,7 @@
     </row>
     <row r="7" spans="1:54" x14ac:dyDescent="0.25">
       <c r="E7" s="4"/>
-      <c r="F7" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="3"/>
       <c r="I7" s="1"/>
@@ -2215,9 +2201,7 @@
     </row>
     <row r="8" spans="1:54" x14ac:dyDescent="0.25">
       <c r="E8" s="4"/>
-      <c r="F8" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="3"/>
       <c r="I8" s="1"/>
@@ -2226,9 +2210,7 @@
     </row>
     <row r="9" spans="1:54" x14ac:dyDescent="0.25">
       <c r="E9" s="4"/>
-      <c r="F9" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="3"/>
       <c r="I9" s="1"/>
@@ -2348,7 +2330,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47C9561B-5C31-4F54-9526-8B42AEE30216}">
   <dimension ref="A1:BB18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2421,7 +2406,7 @@
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="8" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -2533,10 +2518,10 @@
     </row>
     <row r="6" spans="1:54" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G6" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H6" t="s">
         <v>4</v>
@@ -2633,8 +2618,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6F0B329-A77C-4A09-A2FE-86C78D1F79E7}">
   <dimension ref="A1:BB18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11:N11"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2646,6 +2632,7 @@
     <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="24" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:54" s="7" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2709,7 +2696,7 @@
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="8" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -2833,7 +2820,7 @@
         <v>6</v>
       </c>
       <c r="J6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K6" t="s">
         <v>14</v>
@@ -2844,9 +2831,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
-      <c r="J7" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="J7" s="1"/>
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:54" x14ac:dyDescent="0.25">
@@ -2854,9 +2839,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
-      <c r="J8" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="J8" s="1"/>
       <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:54" x14ac:dyDescent="0.25">
@@ -2864,9 +2847,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
-      <c r="J9" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="J9" s="1"/>
       <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:54" x14ac:dyDescent="0.25">
@@ -2953,7 +2934,7 @@
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J7:J18" xr:uid="{2925EAA5-0E84-400E-8FE6-5764D6680FD2}">
       <formula1>"OK,Atenção,Crítico"</formula1>
     </dataValidation>

</xml_diff>